<commit_message>
Working on 1b almost finished
</commit_message>
<xml_diff>
--- a/Data/testWoodcarb.xlsx
+++ b/Data/testWoodcarb.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="0" windowWidth="25360" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="4635" yWindow="0" windowWidth="25365" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -171,9 +171,6 @@
     <t>usa_BL</t>
   </si>
   <si>
-    <t>Var1a_STOCKCHANGE_TOTAL</t>
-  </si>
-  <si>
     <t>Var1b_STOCKCHANGE_TOTAL</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   <si>
     <t>hSP</t>
   </si>
+  <si>
+    <t>Var1_totalC_Output</t>
+  </si>
 </sst>
 </file>
 
@@ -281,6 +281,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -608,20 +613,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU152"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BL2" sqref="BL2:BL152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="64" max="64" width="25.6640625" customWidth="1"/>
-    <col min="65" max="65" width="23.83203125" customWidth="1"/>
+    <col min="64" max="64" width="25.625" customWidth="1"/>
+    <col min="65" max="65" width="23.875" customWidth="1"/>
     <col min="66" max="66" width="31.5" customWidth="1"/>
-    <col min="67" max="67" width="25.1640625" customWidth="1"/>
+    <col min="67" max="67" width="25.125" customWidth="1"/>
     <col min="73" max="73" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +652,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -668,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -680,31 +685,31 @@
         <v>14</v>
       </c>
       <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>63</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>64</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>65</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>69</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>70</v>
       </c>
       <c r="AC1" t="s">
         <v>17</v>
@@ -806,43 +811,43 @@
         <v>49</v>
       </c>
       <c r="BJ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
-        <v>61</v>
-      </c>
       <c r="BL1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BM1" t="s">
         <v>50</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BO1" t="s">
         <v>51</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>53</v>
       </c>
-      <c r="BO1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>54</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>55</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>56</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>57</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>58</v>
       </c>
-      <c r="BU1" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="2" spans="1:73">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1900</v>
       </c>
@@ -1026,8 +1031,11 @@
       <c r="BK2">
         <v>389656843.19585478</v>
       </c>
+      <c r="BL2">
+        <v>5861772.4768134877</v>
+      </c>
     </row>
-    <row r="3" spans="1:73">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1901</v>
       </c>
@@ -1211,8 +1219,11 @@
       <c r="BK3">
         <v>437223238.72604603</v>
       </c>
+      <c r="BL3">
+        <v>11107207.699530974</v>
+      </c>
     </row>
-    <row r="4" spans="1:73">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1902</v>
       </c>
@@ -1396,8 +1407,11 @@
       <c r="BK4">
         <v>485815953.94297212</v>
       </c>
+      <c r="BL4">
+        <v>12110973.317942418</v>
+      </c>
     </row>
-    <row r="5" spans="1:73">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1903</v>
       </c>
@@ -1581,8 +1595,11 @@
       <c r="BK5">
         <v>535634773.92423928</v>
       </c>
+      <c r="BL5">
+        <v>13088917.898367032</v>
+      </c>
     </row>
-    <row r="6" spans="1:73">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1904</v>
       </c>
@@ -1766,8 +1783,11 @@
       <c r="BK6">
         <v>586323753.03475094</v>
       </c>
+      <c r="BL6">
+        <v>14079955.044636741</v>
+      </c>
     </row>
-    <row r="7" spans="1:73">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1905</v>
       </c>
@@ -1951,8 +1971,11 @@
       <c r="BK7">
         <v>637147075.62747848</v>
       </c>
+      <c r="BL7">
+        <v>15038869.737551011</v>
+      </c>
     </row>
-    <row r="8" spans="1:73">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1906</v>
       </c>
@@ -2136,8 +2159,11 @@
       <c r="BK8">
         <v>691452875.15862989</v>
       </c>
+      <c r="BL8">
+        <v>16355132.155010484</v>
+      </c>
     </row>
-    <row r="9" spans="1:73">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1907</v>
       </c>
@@ -2321,8 +2347,11 @@
       <c r="BK9">
         <v>748996033.5582974</v>
       </c>
+      <c r="BL9">
+        <v>17696343.05710458</v>
+      </c>
     </row>
-    <row r="10" spans="1:73">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1908</v>
       </c>
@@ -2506,8 +2535,11 @@
       <c r="BK10">
         <v>799751991.57193506</v>
       </c>
+      <c r="BL10">
+        <v>17980914.267286956</v>
+      </c>
     </row>
-    <row r="11" spans="1:73">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1909</v>
       </c>
@@ -2691,8 +2723,11 @@
       <c r="BK11">
         <v>853415692.07252181</v>
       </c>
+      <c r="BL11">
+        <v>19247980.76036144</v>
+      </c>
     </row>
-    <row r="12" spans="1:73">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1910</v>
       </c>
@@ -2876,8 +2911,11 @@
       <c r="BK12">
         <v>906491919.83012581</v>
       </c>
+      <c r="BL12">
+        <v>20121398.878286839</v>
+      </c>
     </row>
-    <row r="13" spans="1:73">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1911</v>
       </c>
@@ -3061,8 +3099,11 @@
       <c r="BK13">
         <v>956615441.27641511</v>
       </c>
+      <c r="BL13">
+        <v>20691086.233655393</v>
+      </c>
     </row>
-    <row r="14" spans="1:73">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1912</v>
       </c>
@@ -3246,8 +3287,11 @@
       <c r="BK14">
         <v>1007491363.0212278</v>
       </c>
+      <c r="BL14">
+        <v>21664567.954973303</v>
+      </c>
     </row>
-    <row r="15" spans="1:73">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1913</v>
       </c>
@@ -3431,8 +3475,11 @@
       <c r="BK15">
         <v>1056357941.4937975</v>
       </c>
+      <c r="BL15">
+        <v>22326768.209028967</v>
+      </c>
     </row>
-    <row r="16" spans="1:73">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1914</v>
       </c>
@@ -3616,8 +3663,11 @@
       <c r="BK16">
         <v>1100437295.5076444</v>
       </c>
+      <c r="BL16">
+        <v>22734845.238919772</v>
+      </c>
     </row>
-    <row r="17" spans="1:63">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1915</v>
       </c>
@@ -3801,8 +3851,11 @@
       <c r="BK17">
         <v>1139971857.9019358</v>
       </c>
+      <c r="BL17">
+        <v>23095793.93124678</v>
+      </c>
     </row>
-    <row r="18" spans="1:63">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1916</v>
       </c>
@@ -3989,8 +4042,11 @@
       <c r="BK18">
         <v>1181979729.3363106</v>
       </c>
+      <c r="BL18">
+        <v>24126564.668017589</v>
+      </c>
     </row>
-    <row r="19" spans="1:63">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1917</v>
       </c>
@@ -4177,8 +4233,11 @@
       <c r="BK19">
         <v>1219510919.5704572</v>
       </c>
+      <c r="BL19">
+        <v>24394910.870130464</v>
+      </c>
     </row>
-    <row r="20" spans="1:63">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1918</v>
       </c>
@@ -4365,8 +4424,11 @@
       <c r="BK20">
         <v>1253160421.9499819</v>
       </c>
+      <c r="BL20">
+        <v>24651180.615362965</v>
+      </c>
     </row>
-    <row r="21" spans="1:63">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1919</v>
       </c>
@@ -4553,8 +4615,11 @@
       <c r="BK21">
         <v>1288627890.091064</v>
       </c>
+      <c r="BL21">
+        <v>25435542.248658709</v>
+      </c>
     </row>
-    <row r="22" spans="1:63">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1920</v>
       </c>
@@ -4741,8 +4806,11 @@
       <c r="BK22">
         <v>1323564806.9639084</v>
       </c>
+      <c r="BL22">
+        <v>26031574.055885121</v>
+      </c>
     </row>
-    <row r="23" spans="1:63">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1921</v>
       </c>
@@ -4929,8 +4997,11 @@
       <c r="BK23">
         <v>1350343998.8898625</v>
       </c>
+      <c r="BL23">
+        <v>25729505.444059506</v>
+      </c>
     </row>
-    <row r="24" spans="1:63">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1922</v>
       </c>
@@ -5117,8 +5188,11 @@
       <c r="BK24">
         <v>1381418710.5846422</v>
       </c>
+      <c r="BL24">
+        <v>26711456.699059509</v>
+      </c>
     </row>
-    <row r="25" spans="1:63">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1923</v>
       </c>
@@ -5305,8 +5379,11 @@
       <c r="BK25">
         <v>1417143003.1317844</v>
       </c>
+      <c r="BL25">
+        <v>27795700.508901119</v>
+      </c>
     </row>
-    <row r="26" spans="1:63">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1924</v>
       </c>
@@ -5493,8 +5570,11 @@
       <c r="BK26">
         <v>1450595037.0048509</v>
       </c>
+      <c r="BL26">
+        <v>28133640.416426435</v>
+      </c>
     </row>
-    <row r="27" spans="1:63">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1925</v>
       </c>
@@ -5681,8 +5761,11 @@
       <c r="BK27">
         <v>1482453121.647876</v>
       </c>
+      <c r="BL27">
+        <v>28565920.361884296</v>
+      </c>
     </row>
-    <row r="28" spans="1:63">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1926</v>
       </c>
@@ -5869,8 +5952,11 @@
       <c r="BK28">
         <v>1512832806.6109838</v>
       </c>
+      <c r="BL28">
+        <v>28950774.756160446</v>
+      </c>
     </row>
-    <row r="29" spans="1:63">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1927</v>
       </c>
@@ -6060,8 +6146,11 @@
       <c r="BK29">
         <v>1540024013.3976495</v>
       </c>
+      <c r="BL29">
+        <v>29087843.84363357</v>
+      </c>
     </row>
-    <row r="30" spans="1:63">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1928</v>
       </c>
@@ -6251,8 +6340,11 @@
       <c r="BK30">
         <v>1565588909.9124417</v>
       </c>
+      <c r="BL30">
+        <v>29332806.683907479</v>
+      </c>
     </row>
-    <row r="31" spans="1:63">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1929</v>
       </c>
@@ -6442,8 +6534,11 @@
       <c r="BK31">
         <v>1592791071.9514647</v>
       </c>
+      <c r="BL31">
+        <v>29966783.942997802</v>
+      </c>
     </row>
-    <row r="32" spans="1:63">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1930</v>
       </c>
@@ -6633,8 +6728,11 @@
       <c r="BK32">
         <v>1609106006.6319568</v>
       </c>
+      <c r="BL32">
+        <v>29244107.445718028</v>
+      </c>
     </row>
-    <row r="33" spans="1:63">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1931</v>
       </c>
@@ -6824,8 +6922,11 @@
       <c r="BK33">
         <v>1614126694.6971664</v>
       </c>
+      <c r="BL33">
+        <v>28258762.940532029</v>
+      </c>
     </row>
-    <row r="34" spans="1:63">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1932</v>
       </c>
@@ -7015,8 +7116,11 @@
       <c r="BK34">
         <v>1611702856.9412575</v>
       </c>
+      <c r="BL34">
+        <v>27507905.550222665</v>
+      </c>
     </row>
-    <row r="35" spans="1:63">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1933</v>
       </c>
@@ -7206,8 +7310,11 @@
       <c r="BK35">
         <v>1612438748.3344707</v>
       </c>
+      <c r="BL35">
+        <v>27789212.677103274</v>
+      </c>
     </row>
-    <row r="36" spans="1:63">
+    <row r="36" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1934</v>
       </c>
@@ -7397,8 +7504,11 @@
       <c r="BK36">
         <v>1615109724.0843306</v>
       </c>
+      <c r="BL36">
+        <v>27990556.903467514</v>
+      </c>
     </row>
-    <row r="37" spans="1:63">
+    <row r="37" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1935</v>
       </c>
@@ -7588,8 +7698,11 @@
       <c r="BK37">
         <v>1621669227.3154974</v>
       </c>
+      <c r="BL37">
+        <v>28472006.006601132</v>
+      </c>
     </row>
-    <row r="38" spans="1:63">
+    <row r="38" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1936</v>
       </c>
@@ -7779,8 +7892,11 @@
       <c r="BK38">
         <v>1633233879.7525551</v>
       </c>
+      <c r="BL38">
+        <v>29159552.032543812</v>
+      </c>
     </row>
-    <row r="39" spans="1:63">
+    <row r="39" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1937</v>
       </c>
@@ -7970,8 +8086,11 @@
       <c r="BK39">
         <v>1646435001.1792781</v>
       </c>
+      <c r="BL39">
+        <v>29527268.53764116</v>
+      </c>
     </row>
-    <row r="40" spans="1:63">
+    <row r="40" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1938</v>
       </c>
@@ -8161,8 +8280,11 @@
       <c r="BK40">
         <v>1654525776.4670565</v>
       </c>
+      <c r="BL40">
+        <v>29211564.667539142</v>
+      </c>
     </row>
-    <row r="41" spans="1:63">
+    <row r="41" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1939</v>
       </c>
@@ -8352,8 +8474,11 @@
       <c r="BK41">
         <v>1666506225.7275274</v>
       </c>
+      <c r="BL41">
+        <v>29791413.629526764</v>
+      </c>
     </row>
-    <row r="42" spans="1:63">
+    <row r="42" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1940</v>
       </c>
@@ -8543,8 +8668,11 @@
       <c r="BK42">
         <v>1680279603.4842005</v>
       </c>
+      <c r="BL42">
+        <v>30208278.488520101</v>
+      </c>
     </row>
-    <row r="43" spans="1:63">
+    <row r="43" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1941</v>
       </c>
@@ -8734,8 +8862,11 @@
       <c r="BK43">
         <v>1699869288.059917</v>
       </c>
+      <c r="BL43">
+        <v>31173817.404996552</v>
+      </c>
     </row>
-    <row r="44" spans="1:63">
+    <row r="44" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1942</v>
       </c>
@@ -8925,8 +9056,11 @@
       <c r="BK44">
         <v>1718999923.6333818</v>
       </c>
+      <c r="BL44">
+        <v>31504703.182076447</v>
+      </c>
     </row>
-    <row r="45" spans="1:63">
+    <row r="45" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1943</v>
       </c>
@@ -9116,8 +9250,11 @@
       <c r="BK45">
         <v>1735314952.5593953</v>
       </c>
+      <c r="BL45">
+        <v>31478518.687336091</v>
+      </c>
     </row>
-    <row r="46" spans="1:63">
+    <row r="46" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1944</v>
       </c>
@@ -9307,8 +9444,11 @@
       <c r="BK46">
         <v>1750325153.3065078</v>
       </c>
+      <c r="BL46">
+        <v>31638352.776278842</v>
+      </c>
     </row>
-    <row r="47" spans="1:63">
+    <row r="47" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1945</v>
       </c>
@@ -9498,8 +9638,11 @@
       <c r="BK47">
         <v>1760205914.3968132</v>
       </c>
+      <c r="BL47">
+        <v>31341045.332746103</v>
+      </c>
     </row>
-    <row r="48" spans="1:63">
+    <row r="48" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1946</v>
       </c>
@@ -9689,8 +9832,11 @@
       <c r="BK48">
         <v>1775662444.5789378</v>
       </c>
+      <c r="BL48">
+        <v>32138283.587713186</v>
+      </c>
     </row>
-    <row r="49" spans="1:63">
+    <row r="49" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1947</v>
       </c>
@@ -9880,8 +10026,11 @@
       <c r="BK49">
         <v>1792474326.126893</v>
       </c>
+      <c r="BL49">
+        <v>32502889.082307365</v>
+      </c>
     </row>
-    <row r="50" spans="1:63">
+    <row r="50" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1948</v>
       </c>
@@ -10071,8 +10220,11 @@
       <c r="BK50">
         <v>1809173298.4365511</v>
       </c>
+      <c r="BL50">
+        <v>32906201.019293368</v>
+      </c>
     </row>
-    <row r="51" spans="1:63">
+    <row r="51" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1949</v>
       </c>
@@ -10262,8 +10414,11 @@
       <c r="BK51">
         <v>1819492168.0190277</v>
       </c>
+      <c r="BL51">
+        <v>32470431.400846072</v>
+      </c>
     </row>
-    <row r="52" spans="1:63">
+    <row r="52" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1950</v>
       </c>
@@ -10453,8 +10608,11 @@
       <c r="BK52">
         <v>1835029595.0470643</v>
       </c>
+      <c r="BL52">
+        <v>33436502.743709818</v>
+      </c>
     </row>
-    <row r="53" spans="1:63">
+    <row r="53" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1951</v>
       </c>
@@ -10644,8 +10802,11 @@
       <c r="BK53">
         <v>1847623592.7745445</v>
       </c>
+      <c r="BL53">
+        <v>36068772.551706925</v>
+      </c>
     </row>
-    <row r="54" spans="1:63">
+    <row r="54" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1952</v>
       </c>
@@ -10835,8 +10996,11 @@
       <c r="BK54">
         <v>1859739145.9743848</v>
       </c>
+      <c r="BL54">
+        <v>36195276.529252745</v>
+      </c>
     </row>
-    <row r="55" spans="1:63">
+    <row r="55" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1953</v>
       </c>
@@ -11026,8 +11190,11 @@
       <c r="BK55">
         <v>1871360581.6414549</v>
       </c>
+      <c r="BL55">
+        <v>36359525.320088685</v>
+      </c>
     </row>
-    <row r="56" spans="1:63">
+    <row r="56" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1954</v>
       </c>
@@ -11217,8 +11384,11 @@
       <c r="BK56">
         <v>1882349761.9673543</v>
       </c>
+      <c r="BL56">
+        <v>36495513.217898309</v>
+      </c>
     </row>
-    <row r="57" spans="1:63">
+    <row r="57" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1955</v>
       </c>
@@ -11408,8 +11578,11 @@
       <c r="BK57">
         <v>1894761766.7395563</v>
       </c>
+      <c r="BL57">
+        <v>36845888.368946053</v>
+      </c>
     </row>
-    <row r="58" spans="1:63">
+    <row r="58" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1956</v>
       </c>
@@ -11599,8 +11772,11 @@
       <c r="BK58">
         <v>1907595878.6065559</v>
       </c>
+      <c r="BL58">
+        <v>37079812.52549763</v>
+      </c>
     </row>
-    <row r="59" spans="1:63">
+    <row r="59" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1957</v>
       </c>
@@ -11790,8 +11966,11 @@
       <c r="BK59">
         <v>1915011592.0775523</v>
       </c>
+      <c r="BL59">
+        <v>36638889.516439773</v>
+      </c>
     </row>
-    <row r="60" spans="1:63">
+    <row r="60" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1958</v>
       </c>
@@ -11981,8 +12160,11 @@
       <c r="BK60">
         <v>1923104451.2515507</v>
       </c>
+      <c r="BL60">
+        <v>36851418.178238228</v>
+      </c>
     </row>
-    <row r="61" spans="1:63">
+    <row r="61" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1959</v>
       </c>
@@ -12172,8 +12354,11 @@
       <c r="BK61">
         <v>1934798390.6792412</v>
       </c>
+      <c r="BL61">
+        <v>37433299.215469189</v>
+      </c>
     </row>
-    <row r="62" spans="1:63">
+    <row r="62" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1960</v>
       </c>
@@ -12363,8 +12548,11 @@
       <c r="BK62">
         <v>1942504009.904635</v>
       </c>
+      <c r="BL62">
+        <v>37140892.939016894</v>
+      </c>
     </row>
-    <row r="63" spans="1:63">
+    <row r="63" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1961</v>
       </c>
@@ -12554,8 +12742,11 @@
       <c r="BK63">
         <v>1949817585.3592472</v>
       </c>
+      <c r="BL63">
+        <v>37206736.84893553</v>
+      </c>
     </row>
-    <row r="64" spans="1:63">
+    <row r="64" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1962</v>
       </c>
@@ -12745,8 +12936,11 @@
       <c r="BK64">
         <v>1958417521.6428785</v>
       </c>
+      <c r="BL64">
+        <v>37525614.063833527</v>
+      </c>
     </row>
-    <row r="65" spans="1:63">
+    <row r="65" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1963</v>
       </c>
@@ -12936,8 +13130,11 @@
       <c r="BK65">
         <v>1970302941.1726561</v>
       </c>
+      <c r="BL65">
+        <v>38008001.577397153</v>
+      </c>
     </row>
-    <row r="66" spans="1:63">
+    <row r="66" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1964</v>
       </c>
@@ -13127,8 +13324,11 @@
       <c r="BK66">
         <v>1984776231.593184</v>
       </c>
+      <c r="BL66">
+        <v>38461416.73345612</v>
+      </c>
     </row>
-    <row r="67" spans="1:63">
+    <row r="67" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1965</v>
       </c>
@@ -13318,8 +13518,11 @@
       <c r="BK67">
         <v>2002330065.4513638</v>
       </c>
+      <c r="BL67">
+        <v>39047040.816286109</v>
+      </c>
     </row>
-    <row r="68" spans="1:63">
+    <row r="68" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1966</v>
       </c>
@@ -13509,8 +13712,11 @@
       <c r="BK68">
         <v>2020358747.4500315</v>
       </c>
+      <c r="BL68">
+        <v>39370990.825217731</v>
+      </c>
     </row>
-    <row r="69" spans="1:63">
+    <row r="69" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1967</v>
       </c>
@@ -13700,8 +13906,11 @@
       <c r="BK69">
         <v>2037009049.3629086</v>
       </c>
+      <c r="BL69">
+        <v>39450416.506517678</v>
+      </c>
     </row>
-    <row r="70" spans="1:63">
+    <row r="70" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1968</v>
       </c>
@@ -13891,8 +14100,11 @@
       <c r="BK70">
         <v>2055467575.9731295</v>
       </c>
+      <c r="BL70">
+        <v>39999080.230682567</v>
+      </c>
     </row>
-    <row r="71" spans="1:63">
+    <row r="71" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1969</v>
       </c>
@@ -14082,8 +14294,11 @@
       <c r="BK71">
         <v>2073967142.3924487</v>
       </c>
+      <c r="BL71">
+        <v>40367458.604179874</v>
+      </c>
     </row>
-    <row r="72" spans="1:63">
+    <row r="72" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1970</v>
       </c>
@@ -14273,8 +14488,11 @@
       <c r="BK72">
         <v>2092043818.3584888</v>
       </c>
+      <c r="BL72">
+        <v>40615735.003486946</v>
+      </c>
     </row>
-    <row r="73" spans="1:63">
+    <row r="73" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1971</v>
       </c>
@@ -14464,8 +14682,11 @@
       <c r="BK73">
         <v>2113169051.5297117</v>
       </c>
+      <c r="BL73">
+        <v>41440882.010553926</v>
+      </c>
     </row>
-    <row r="74" spans="1:63">
+    <row r="74" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1972</v>
       </c>
@@ -14655,8 +14876,11 @@
       <c r="BK74">
         <v>2136141832.7466304</v>
       </c>
+      <c r="BL74">
+        <v>42120218.771336287</v>
+      </c>
     </row>
-    <row r="75" spans="1:63">
+    <row r="75" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1973</v>
       </c>
@@ -14846,8 +15070,11 @@
       <c r="BK75">
         <v>2159881024.4835129</v>
       </c>
+      <c r="BL75">
+        <v>42552082.222033814</v>
+      </c>
     </row>
-    <row r="76" spans="1:63">
+    <row r="76" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1974</v>
       </c>
@@ -15037,8 +15264,11 @@
       <c r="BK76">
         <v>2176368934.0413551</v>
       </c>
+      <c r="BL76">
+        <v>42056278.70604521</v>
+      </c>
     </row>
-    <row r="77" spans="1:63">
+    <row r="77" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1975</v>
       </c>
@@ -15228,8 +15458,11 @@
       <c r="BK77">
         <v>2189142648.2544675</v>
       </c>
+      <c r="BL77">
+        <v>41848275.269384481</v>
+      </c>
     </row>
-    <row r="78" spans="1:63">
+    <row r="78" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1976</v>
       </c>
@@ -15419,8 +15652,11 @@
       <c r="BK78">
         <v>2207530466.9861155</v>
       </c>
+      <c r="BL78">
+        <v>42797261.404742464</v>
+      </c>
     </row>
-    <row r="79" spans="1:63">
+    <row r="79" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1977</v>
       </c>
@@ -15610,8 +15846,11 @@
       <c r="BK79">
         <v>2228948878.0906224</v>
       </c>
+      <c r="BL79">
+        <v>43745152.40859618</v>
+      </c>
     </row>
-    <row r="80" spans="1:63">
+    <row r="80" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1978</v>
       </c>
@@ -15801,8 +16040,11 @@
       <c r="BK80">
         <v>2251850142.0838919</v>
       </c>
+      <c r="BL80">
+        <v>44434610.698394954</v>
+      </c>
     </row>
-    <row r="81" spans="1:73">
+    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1979</v>
       </c>
@@ -15992,8 +16234,11 @@
       <c r="BK81">
         <v>2274348137.5880699</v>
       </c>
+      <c r="BL81">
+        <v>44712739.419059835</v>
+      </c>
     </row>
-    <row r="82" spans="1:73">
+    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1980</v>
       </c>
@@ -16183,8 +16428,11 @@
       <c r="BK82">
         <v>2289667985.6178951</v>
       </c>
+      <c r="BL82">
+        <v>44230154.241114073</v>
+      </c>
     </row>
-    <row r="83" spans="1:73">
+    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1981</v>
       </c>
@@ -16374,8 +16622,11 @@
       <c r="BK83">
         <v>2300960774.4692373</v>
       </c>
+      <c r="BL83">
+        <v>44127601.905859753</v>
+      </c>
     </row>
-    <row r="84" spans="1:73">
+    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1982</v>
       </c>
@@ -16565,8 +16816,11 @@
       <c r="BK84">
         <v>2311957218.6760106</v>
       </c>
+      <c r="BL84">
+        <v>44363783.162989564</v>
+      </c>
     </row>
-    <row r="85" spans="1:73">
+    <row r="85" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1983</v>
       </c>
@@ -16756,8 +17010,11 @@
       <c r="BK85">
         <v>2331904123.0040159</v>
       </c>
+      <c r="BL85">
+        <v>45804828.860371761</v>
+      </c>
     </row>
-    <row r="86" spans="1:73">
+    <row r="86" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1984</v>
       </c>
@@ -16947,8 +17204,11 @@
       <c r="BK86">
         <v>2355133348.820817</v>
       </c>
+      <c r="BL86">
+        <v>46769358.424599171</v>
+      </c>
     </row>
-    <row r="87" spans="1:73">
+    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1985</v>
       </c>
@@ -17138,8 +17398,11 @@
       <c r="BK87">
         <v>2378443226.4848413</v>
       </c>
+      <c r="BL87">
+        <v>47427273.101053461</v>
+      </c>
     </row>
-    <row r="88" spans="1:73">
+    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1986</v>
       </c>
@@ -17329,8 +17592,11 @@
       <c r="BK88">
         <v>2406795969.2063608</v>
       </c>
+      <c r="BL88">
+        <v>48444305.917312309</v>
+      </c>
     </row>
-    <row r="89" spans="1:73">
+    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1987</v>
       </c>
@@ -17520,8 +17786,11 @@
       <c r="BK89">
         <v>2439433712.8990016</v>
       </c>
+      <c r="BL89">
+        <v>49502786.917974636</v>
+      </c>
     </row>
-    <row r="90" spans="1:73">
+    <row r="90" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1988</v>
       </c>
@@ -17711,8 +17980,11 @@
       <c r="BK90">
         <v>2473277026.2187462</v>
       </c>
+      <c r="BL90">
+        <v>49952927.46418637</v>
+      </c>
     </row>
-    <row r="91" spans="1:73">
+    <row r="91" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1989</v>
       </c>
@@ -17902,8 +18174,11 @@
       <c r="BK91">
         <v>2507032595.7482305</v>
       </c>
+      <c r="BL91">
+        <v>50512852.148384809</v>
+      </c>
     </row>
-    <row r="92" spans="1:73">
+    <row r="92" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1990</v>
       </c>
@@ -18094,7 +18369,7 @@
         <v>2538693596.6428919</v>
       </c>
       <c r="BL92">
-        <v>17043.711617142661</v>
+        <v>50789440.409271389</v>
       </c>
       <c r="BM92">
         <v>18307.633544483891</v>
@@ -18124,7 +18399,7 @@
         <v>-131771.55498549016</v>
       </c>
     </row>
-    <row r="93" spans="1:73">
+    <row r="93" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1991</v>
       </c>
@@ -18315,7 +18590,7 @@
         <v>2564882702.4099097</v>
       </c>
       <c r="BL93">
-        <v>13128.824896964934</v>
+        <v>50653922.480584003</v>
       </c>
       <c r="BM93">
         <v>18601.567111390792</v>
@@ -18345,7 +18620,7 @@
         <v>-123758.01437821392</v>
       </c>
     </row>
-    <row r="94" spans="1:73">
+    <row r="94" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1992</v>
       </c>
@@ -18536,7 +18811,7 @@
         <v>2592740383.1683764</v>
       </c>
       <c r="BL94">
-        <v>15717.73916917243</v>
+        <v>51521203.174823865</v>
       </c>
       <c r="BM94">
         <v>17005.5189498869</v>
@@ -18566,7 +18841,7 @@
         <v>-123790.60574321589</v>
       </c>
     </row>
-    <row r="95" spans="1:73">
+    <row r="95" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1993</v>
       </c>
@@ -18757,7 +19032,7 @@
         <v>2619668467.918571</v>
       </c>
       <c r="BL95">
-        <v>16956.723267507528</v>
+        <v>52205308.524761304</v>
       </c>
       <c r="BM95">
         <v>17626.582923235732</v>
@@ -18787,7 +19062,7 @@
         <v>-120707.518895416</v>
       </c>
     </row>
-    <row r="96" spans="1:73">
+    <row r="96" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1994</v>
       </c>
@@ -18978,7 +19253,7 @@
         <v>2646393294.2087274</v>
       </c>
       <c r="BL96">
-        <v>18220.972549406419</v>
+        <v>52891672.850889988</v>
       </c>
       <c r="BM96">
         <v>17220.927687487256</v>
@@ -19008,7 +19283,7 @@
         <v>-122498.30707318462</v>
       </c>
     </row>
-    <row r="97" spans="1:73">
+    <row r="97" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1995</v>
       </c>
@@ -19199,7 +19474,7 @@
         <v>2671160602.8903418</v>
       </c>
       <c r="BL97">
-        <v>17306.863251957609</v>
+        <v>53352870.286617175</v>
       </c>
       <c r="BM97">
         <v>17051.465656525332</v>
@@ -19229,7 +19504,7 @@
         <v>-118411.13044839063</v>
       </c>
     </row>
-    <row r="98" spans="1:73">
+    <row r="98" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1996</v>
       </c>
@@ -19420,7 +19695,7 @@
         <v>2696430161.2166786</v>
       </c>
       <c r="BL98">
-        <v>17018.001126356696</v>
+        <v>54077914.362575822</v>
       </c>
       <c r="BM98">
         <v>16347.531752535033</v>
@@ -19450,7 +19725,7 @@
         <v>-112219.09920656984</v>
       </c>
     </row>
-    <row r="99" spans="1:73">
+    <row r="99" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1997</v>
       </c>
@@ -19641,7 +19916,7 @@
         <v>2722349173.0367541</v>
       </c>
       <c r="BL99">
-        <v>18755.628978591256</v>
+        <v>54787478.003478453</v>
       </c>
       <c r="BM99">
         <v>17090.104072172864</v>
@@ -19671,7 +19946,7 @@
         <v>-117343.82567911665</v>
       </c>
     </row>
-    <row r="100" spans="1:73">
+    <row r="100" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1998</v>
       </c>
@@ -19862,7 +20137,7 @@
         <v>2747440883.7917299</v>
       </c>
       <c r="BL100">
-        <v>19653.677269110267</v>
+        <v>55587859.252851486</v>
       </c>
       <c r="BM100">
         <v>17769.367702534139</v>
@@ -19892,7 +20167,7 @@
         <v>-114188.44514703227</v>
       </c>
     </row>
-    <row r="101" spans="1:73">
+    <row r="101" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1999</v>
       </c>
@@ -20083,7 +20358,7 @@
         <v>2774210114.167881</v>
       </c>
       <c r="BL101">
-        <v>21444.227703879114</v>
+        <v>56476870.788903393</v>
       </c>
       <c r="BM101">
         <v>18662.301475814074</v>
@@ -20113,7 +20388,7 @@
         <v>-119182.37215582242</v>
       </c>
     </row>
-    <row r="102" spans="1:73">
+    <row r="102" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2000</v>
       </c>
@@ -20304,7 +20579,7 @@
         <v>2800357395.2847004</v>
       </c>
       <c r="BL102">
-        <v>19999.515374209102</v>
+        <v>57095558.678844079</v>
       </c>
       <c r="BM102">
         <v>18508.291885005783</v>
@@ -20334,7 +20609,7 @@
         <v>-112968.80442999951</v>
       </c>
     </row>
-    <row r="103" spans="1:73">
+    <row r="103" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2001</v>
       </c>
@@ -20525,7 +20800,7 @@
         <v>2822573761.8943901</v>
       </c>
       <c r="BL103">
-        <v>16491.42940879834</v>
+        <v>57475588.403711736</v>
       </c>
       <c r="BM103">
         <v>17610.238639237592</v>
@@ -20555,7 +20830,7 @@
         <v>-93478.727368143052</v>
       </c>
     </row>
-    <row r="104" spans="1:73">
+    <row r="104" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2002</v>
       </c>
@@ -20746,7 +21021,7 @@
         <v>2846096428.5869803</v>
       </c>
       <c r="BL104">
-        <v>17413.829817791993</v>
+        <v>58306899.410335012</v>
       </c>
       <c r="BM104">
         <v>18235.446752712014</v>
@@ -20776,7 +21051,7 @@
         <v>-98188.126908603066</v>
       </c>
     </row>
-    <row r="105" spans="1:73">
+    <row r="105" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2003</v>
       </c>
@@ -20967,7 +21242,7 @@
         <v>2867921752.3019114</v>
       </c>
       <c r="BL105">
-        <v>16986.418531517393</v>
+        <v>58878410.969623826</v>
       </c>
       <c r="BM105">
         <v>17325.96486346746</v>
@@ -20997,7 +21272,7 @@
         <v>-93967.400095627934</v>
       </c>
     </row>
-    <row r="106" spans="1:73">
+    <row r="106" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2004</v>
       </c>
@@ -21188,7 +21463,7 @@
         <v>2892776889.2836533</v>
       </c>
       <c r="BL106">
-        <v>21409.198256646931</v>
+        <v>60241447.722770736</v>
       </c>
       <c r="BM106">
         <v>17643.503019332067</v>
@@ -21218,7 +21493,7 @@
         <v>-103967.46194377833</v>
       </c>
     </row>
-    <row r="107" spans="1:73">
+    <row r="107" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2005</v>
       </c>
@@ -21409,7 +21684,7 @@
         <v>2917679759.8848152</v>
       </c>
       <c r="BL107">
-        <v>20989.891865423793</v>
+        <v>61080815.078452639</v>
       </c>
       <c r="BM107">
         <v>17765.220093910139</v>
@@ -21439,7 +21714,7 @@
         <v>-102683.1743462734</v>
       </c>
     </row>
-    <row r="108" spans="1:73">
+    <row r="108" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2006</v>
       </c>
@@ -21630,7 +21905,7 @@
         <v>2940765110.2871881</v>
       </c>
       <c r="BL108">
-        <v>19082.752088916179</v>
+        <v>61324266.776435003</v>
       </c>
       <c r="BM108">
         <v>18586.792318825137</v>
@@ -21660,7 +21935,7 @@
         <v>-107666.14366573984</v>
       </c>
     </row>
-    <row r="109" spans="1:73">
+    <row r="109" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2007</v>
       </c>
@@ -21851,7 +22126,7 @@
         <v>2959512311.6914454</v>
       </c>
       <c r="BL109">
-        <v>13091.542600677052</v>
+        <v>60853366.689290695</v>
       </c>
       <c r="BM109">
         <v>18307.971565376833</v>
@@ -21881,7 +22156,7 @@
         <v>-102762.70036301664</v>
       </c>
     </row>
-    <row r="110" spans="1:73">
+    <row r="110" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2008</v>
       </c>
@@ -22072,7 +22347,7 @@
         <v>2965821012.111145</v>
       </c>
       <c r="BL110">
-        <v>2420.1491721504258</v>
+        <v>59250725.680234902</v>
       </c>
       <c r="BM110">
         <v>17510.544900104152</v>
@@ -22102,7 +22377,7 @@
         <v>-76830.261033082919</v>
       </c>
     </row>
-    <row r="111" spans="1:73">
+    <row r="111" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2009</v>
       </c>
@@ -22293,7 +22568,7 @@
         <v>2964690550.1407099</v>
       </c>
       <c r="BL111">
-        <v>-5103.8429804886009</v>
+        <v>58232242.619164847</v>
       </c>
       <c r="BM111">
         <v>16641.590134239348</v>
@@ -22323,7 +22598,7 @@
         <v>-54360.975636586372</v>
       </c>
     </row>
-    <row r="112" spans="1:73">
+    <row r="112" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2010</v>
       </c>
@@ -22514,7 +22789,7 @@
         <v>2964308017.547183</v>
       </c>
       <c r="BL112">
-        <v>-2895.9387419946497</v>
+        <v>58163727.003920771</v>
       </c>
       <c r="BM112">
         <v>16300.851641078936</v>
@@ -22544,7 +22819,7 @@
         <v>-60549.58261540634</v>
       </c>
     </row>
-    <row r="113" spans="1:73">
+    <row r="113" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2011</v>
       </c>
@@ -22735,7 +23010,7 @@
         <v>2966945773.6524258</v>
       </c>
       <c r="BL113">
-        <v>-1887.2389913888071</v>
+        <v>58298544.497461699</v>
       </c>
       <c r="BM113">
         <v>16171.282500943078</v>
@@ -22765,7 +23040,7 @@
         <v>-68943.222413245952</v>
       </c>
     </row>
-    <row r="114" spans="1:73">
+    <row r="114" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2012</v>
       </c>
@@ -22956,7 +23231,7 @@
         <v>2970683079.1117067</v>
       </c>
       <c r="BL114">
-        <v>-298.55971726283894</v>
+        <v>58507421.308226079</v>
       </c>
       <c r="BM114">
         <v>16112.035297906132</v>
@@ -22986,7 +23261,7 @@
         <v>-68312.971140974638</v>
       </c>
     </row>
-    <row r="115" spans="1:73">
+    <row r="115" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2013</v>
       </c>
@@ -23177,7 +23452,7 @@
         <v>2977443518.8774414</v>
       </c>
       <c r="BL115">
-        <v>2298.3609292553515</v>
+        <v>58959536.607529126</v>
       </c>
       <c r="BM115">
         <v>16188.344345186095</v>
@@ -23207,7 +23482,7 @@
         <v>-70814.784636133685</v>
       </c>
     </row>
-    <row r="116" spans="1:73">
+    <row r="116" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2014</v>
       </c>
@@ -23398,7 +23673,7 @@
         <v>2985851215.9569564</v>
       </c>
       <c r="BL116">
-        <v>12943.668378991997</v>
+        <v>59492926.333034784</v>
       </c>
       <c r="BM116">
         <v>17146.434694848838</v>
@@ -23428,7 +23703,7 @@
         <v>-86538.25988882019</v>
       </c>
     </row>
-    <row r="117" spans="1:73">
+    <row r="117" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2015</v>
       </c>
@@ -23619,7 +23894,7 @@
         <v>2996456638.3327913</v>
       </c>
       <c r="BL117">
-        <v>13474.08685419727</v>
+        <v>60054468.394272581</v>
       </c>
       <c r="BM117">
         <v>17965.441070686258</v>
@@ -23649,7 +23924,7 @@
         <v>-91250.870301594041</v>
       </c>
     </row>
-    <row r="118" spans="1:73">
+    <row r="118" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2016</v>
       </c>
@@ -23840,7 +24115,7 @@
         <v>3009221478.5042706</v>
       </c>
       <c r="BL118">
-        <v>13987.129617475917</v>
+        <v>60680174.483157687</v>
       </c>
       <c r="BM118">
         <v>18662.342308712443</v>
@@ -23870,7 +24145,7 @@
         <v>-94414.371045958367</v>
       </c>
     </row>
-    <row r="119" spans="1:73">
+    <row r="119" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2017</v>
       </c>
@@ -24061,7 +24336,7 @@
         <v>3024108271.5067968</v>
       </c>
       <c r="BL119">
-        <v>15053.10692608536</v>
+        <v>61368780.056006297</v>
       </c>
       <c r="BM119">
         <v>19298.766364838099</v>
@@ -24091,7 +24366,7 @@
         <v>-99002.145690345787</v>
       </c>
     </row>
-    <row r="120" spans="1:73">
+    <row r="120" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2018</v>
       </c>
@@ -24282,7 +24557,7 @@
         <v>3041080365.0354729</v>
       </c>
       <c r="BL120">
-        <v>16122.354439389292</v>
+        <v>62119048.182299905</v>
       </c>
       <c r="BM120">
         <v>19879.951855534076</v>
@@ -24312,7 +24587,7 @@
         <v>-103283.78789374525</v>
       </c>
     </row>
-    <row r="121" spans="1:73">
+    <row r="121" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2019</v>
       </c>
@@ -24503,7 +24778,7 @@
         <v>3060101892.20298</v>
       </c>
       <c r="BL121">
-        <v>17273.201182915458</v>
+        <v>62929768.898728885</v>
       </c>
       <c r="BM121">
         <v>20418.644126021914</v>
@@ -24533,7 +24808,7 @@
         <v>-107677.39546834149</v>
       </c>
     </row>
-    <row r="122" spans="1:73">
+    <row r="122" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2020</v>
       </c>
@@ -24724,7 +24999,7 @@
         <v>3080862962.1888032</v>
       </c>
       <c r="BL122">
-        <v>19912.213811498546</v>
+        <v>64110434.056330606</v>
       </c>
       <c r="BM122">
         <v>21027.110860099423</v>
@@ -24754,7 +25029,7 @@
         <v>-111689.9511899411</v>
       </c>
     </row>
-    <row r="123" spans="1:73">
+    <row r="123" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2021</v>
       </c>
@@ -24938,8 +25213,11 @@
       <c r="BK123">
         <v>3109265319.7730393</v>
       </c>
+      <c r="BL123">
+        <v>65043010.815260977</v>
+      </c>
     </row>
-    <row r="124" spans="1:73">
+    <row r="124" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2022</v>
       </c>
@@ -25123,8 +25401,11 @@
       <c r="BK124">
         <v>3137711385.2582684</v>
       </c>
+      <c r="BL124">
+        <v>65625794.718345448</v>
+      </c>
     </row>
-    <row r="125" spans="1:73">
+    <row r="125" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2023</v>
       </c>
@@ -25308,8 +25589,11 @@
       <c r="BK125">
         <v>3166348249.1337576</v>
       </c>
+      <c r="BL125">
+        <v>66225681.965189941</v>
+      </c>
     </row>
-    <row r="126" spans="1:73">
+    <row r="126" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2024</v>
       </c>
@@ -25493,8 +25777,11 @@
       <c r="BK126">
         <v>3195077805.0832367</v>
       </c>
+      <c r="BL126">
+        <v>66817738.292229086</v>
+      </c>
     </row>
-    <row r="127" spans="1:73">
+    <row r="127" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2025</v>
       </c>
@@ -25678,8 +25965,11 @@
       <c r="BK127">
         <v>3223592823.0698137</v>
       </c>
+      <c r="BL127">
+        <v>67362284.731110185</v>
+      </c>
     </row>
-    <row r="128" spans="1:73">
+    <row r="128" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2026</v>
       </c>
@@ -25863,8 +26153,11 @@
       <c r="BK128">
         <v>3251732534.9123645</v>
       </c>
+      <c r="BL128">
+        <v>67889381.776356235</v>
+      </c>
     </row>
-    <row r="129" spans="1:63">
+    <row r="129" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2027</v>
       </c>
@@ -26048,8 +26341,11 @@
       <c r="BK129">
         <v>3279685709.2633152</v>
       </c>
+      <c r="BL129">
+        <v>68451036.827588499</v>
+      </c>
     </row>
-    <row r="130" spans="1:63">
+    <row r="130" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2028</v>
       </c>
@@ -26233,8 +26529,11 @@
       <c r="BK130">
         <v>3307405040.9677124</v>
       </c>
+      <c r="BL130">
+        <v>68987318.217551723</v>
+      </c>
     </row>
-    <row r="131" spans="1:63">
+    <row r="131" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2029</v>
       </c>
@@ -26418,8 +26717,11 @@
       <c r="BK131">
         <v>3335028954.7768664</v>
       </c>
+      <c r="BL131">
+        <v>69524230.496142685</v>
+      </c>
     </row>
-    <row r="132" spans="1:63">
+    <row r="132" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2030</v>
       </c>
@@ -26603,8 +26905,11 @@
       <c r="BK132">
         <v>3362562630.7032099</v>
       </c>
+      <c r="BL132">
+        <v>70052880.927325845</v>
+      </c>
     </row>
-    <row r="133" spans="1:63">
+    <row r="133" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2031</v>
       </c>
@@ -26788,8 +27093,11 @@
       <c r="BK133">
         <v>3390437565.1407242</v>
       </c>
+      <c r="BL133">
+        <v>70650266.539540887</v>
+      </c>
     </row>
-    <row r="134" spans="1:63">
+    <row r="134" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2032</v>
       </c>
@@ -26973,8 +27281,11 @@
       <c r="BK134">
         <v>3418257821.1067739</v>
       </c>
+      <c r="BL134">
+        <v>71174220.481345162</v>
+      </c>
     </row>
-    <row r="135" spans="1:63">
+    <row r="135" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2033</v>
       </c>
@@ -27158,8 +27469,11 @@
       <c r="BK135">
         <v>3446082442.9488559</v>
       </c>
+      <c r="BL135">
+        <v>71742773.793748215</v>
+      </c>
     </row>
-    <row r="136" spans="1:63">
+    <row r="136" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2034</v>
       </c>
@@ -27343,8 +27657,11 @@
       <c r="BK136">
         <v>3474032478.0715108</v>
       </c>
+      <c r="BL136">
+        <v>72316781.767209962</v>
+      </c>
     </row>
-    <row r="137" spans="1:63">
+    <row r="137" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2035</v>
       </c>
@@ -27528,8 +27845,11 @@
       <c r="BK137">
         <v>3501928117.9174714</v>
       </c>
+      <c r="BL137">
+        <v>72866313.371986657</v>
+      </c>
     </row>
-    <row r="138" spans="1:63">
+    <row r="138" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2036</v>
       </c>
@@ -27713,8 +28033,11 @@
       <c r="BK138">
         <v>3530042534.5184145</v>
       </c>
+      <c r="BL138">
+        <v>73443580.676817179</v>
+      </c>
     </row>
-    <row r="139" spans="1:63">
+    <row r="139" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2037</v>
       </c>
@@ -27898,8 +28221,11 @@
       <c r="BK139">
         <v>3558233763.8585868</v>
       </c>
+      <c r="BL139">
+        <v>73994241.330868781</v>
+      </c>
     </row>
-    <row r="140" spans="1:63">
+    <row r="140" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2038</v>
       </c>
@@ -28083,8 +28409,11 @@
       <c r="BK140">
         <v>3586497650.5681043</v>
       </c>
+      <c r="BL140">
+        <v>74528083.338661656</v>
+      </c>
     </row>
-    <row r="141" spans="1:63">
+    <row r="141" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2039</v>
       </c>
@@ -28268,8 +28597,11 @@
       <c r="BK141">
         <v>3614949742.378037</v>
       </c>
+      <c r="BL141">
+        <v>75080146.843625098</v>
+      </c>
     </row>
-    <row r="142" spans="1:63">
+    <row r="142" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2040</v>
       </c>
@@ -28453,8 +28785,11 @@
       <c r="BK142">
         <v>3643706437.4867463</v>
       </c>
+      <c r="BL142">
+        <v>75653935.344137818</v>
+      </c>
     </row>
-    <row r="143" spans="1:63">
+    <row r="143" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2041</v>
       </c>
@@ -28638,8 +28973,11 @@
       <c r="BK143">
         <v>3672821547.5649023</v>
       </c>
+      <c r="BL143">
+        <v>76236019.02358593</v>
+      </c>
     </row>
-    <row r="144" spans="1:63">
+    <row r="144" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2042</v>
       </c>
@@ -28823,8 +29161,11 @@
       <c r="BK144">
         <v>3702192497.3414698</v>
       </c>
+      <c r="BL144">
+        <v>76843634.577108741</v>
+      </c>
     </row>
-    <row r="145" spans="1:63">
+    <row r="145" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2043</v>
       </c>
@@ -29008,8 +29349,11 @@
       <c r="BK145">
         <v>3731875758.616118</v>
       </c>
+      <c r="BL145">
+        <v>77454777.414531231</v>
+      </c>
     </row>
-    <row r="146" spans="1:63">
+    <row r="146" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2044</v>
       </c>
@@ -29193,8 +29537,11 @@
       <c r="BK146">
         <v>3761767705.4655275</v>
       </c>
+      <c r="BL146">
+        <v>78034271.763398319</v>
+      </c>
     </row>
-    <row r="147" spans="1:63">
+    <row r="147" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2045</v>
       </c>
@@ -29378,8 +29725,11 @@
       <c r="BK147">
         <v>3791890649.3883138</v>
       </c>
+      <c r="BL147">
+        <v>78638964.061451614</v>
+      </c>
     </row>
-    <row r="148" spans="1:63">
+    <row r="148" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2046</v>
       </c>
@@ -29563,8 +29913,11 @@
       <c r="BK148">
         <v>3822152380.5814319</v>
       </c>
+      <c r="BL148">
+        <v>79221218.7722615</v>
+      </c>
     </row>
-    <row r="149" spans="1:63">
+    <row r="149" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2047</v>
       </c>
@@ -29748,8 +30101,11 @@
       <c r="BK149">
         <v>3852674771.0872951</v>
       </c>
+      <c r="BL149">
+        <v>79808372.30424574</v>
+      </c>
     </row>
-    <row r="150" spans="1:63">
+    <row r="150" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2048</v>
       </c>
@@ -29933,8 +30289,11 @@
       <c r="BK150">
         <v>3883393304.2495294</v>
       </c>
+      <c r="BL150">
+        <v>80399049.186338097</v>
+      </c>
     </row>
-    <row r="151" spans="1:63">
+    <row r="151" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2049</v>
       </c>
@@ -30118,8 +30477,11 @@
       <c r="BK151">
         <v>3914401859.1251478</v>
       </c>
+      <c r="BL151">
+        <v>80988190.030189544</v>
+      </c>
     </row>
-    <row r="152" spans="1:63">
+    <row r="152" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2050</v>
       </c>
@@ -30302,6 +30664,9 @@
       </c>
       <c r="BK152">
         <v>3945606868.6721969</v>
+      </c>
+      <c r="BL152">
+        <v>81574096.161355004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>